<commit_message>
all single filter scripts in CTDC
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_AssocFileFormat-Bai.xlsx
+++ b/InputFiles/TC01_Trials_Filter_AssocFileFormat-Bai.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Automation\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E316A51-C398-415D-8298-9957487AFDEA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0C65E9-DB6E-4081-8ED1-32BF520A2429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>WebExcel</t>
   </si>
@@ -51,10 +51,69 @@
     <t>StatQuery</t>
   </si>
   <si>
-    <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report)OPTIONAL MATCH (s)&lt;-[*]-(f:file)  WITH  c AS c, t ,a, s WHERE f.file_format IN ['bai']  RETURN DISTINCT coalesce(c.case_id,'') AS `Case ID` , coalesce(t.clinical_trial_designation ,'')as `Trial Code` , coalesce(a.arm_id,'') As `Arm` , coalesce(a.arm_drug,'') As `Arm Treatment` , coalesce(c.disease,'') As Diagnosis , coalesce(c.gender,'') As Gender , coalesce(c.race,'') As Race , coalesce(c.ethnicity,'') As Ethnicity</t>
-  </si>
-  <si>
-    <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report)OPTIONAL MATCH (s)&lt;-[*]-(f:file)  WITH  c AS c, t ,a, s , f WHERE f.file_format IN ['bai','bam','vcf'] RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(t.clinical_trial_designation)) as number_of_trial</t>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>CasesTab</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (c:case)
+ MATCH (c)-[:of_arm]-&gt;(a:arm)-[:of_trial]-&gt;(ct:clinical_trial)
+ MATCH (f:file)-[*]-&gt;(c)
+WHERE f.file_format IN ['bai'] 
+RETURN DISTINCT
+    c.case_id AS `Case ID`,
+     ct.clinical_trial_designation AS `Trial Code`,
+     a.arm_id AS Arm,
+      a.arm_drug AS `Arm Treatment`,
+c.disease AS Diagnosis,
+  c.gender AS Gender,
+    c.race AS Race,
+    c.ethnicity AS Ethnicity</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)
+OPTIONAL MATCH (f)-[*]-&gt;(a:arm)-[:of_trial]-&gt;(ct:clinical_trial)
+OPTIONAL MATCH (f)-[*]-&gt;(c:case)
+WITH f,a,ct,c
+      WHERE f.file_format IN ['bai'] 
+RETURN
+    COUNT(DISTINCT ct.clinical_trial_designation) AS Trials,
+    COUNT(DISTINCT c.case_id) AS Cases,
+    COUNT(DISTINCT f) AS Files</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)
+OPTIONAL MATCH (f)-[*]-&gt;(a:arm)-[:of_trial]-&gt;(ct:clinical_trial)
+OPTIONAL MATCH (f)-[*]-&gt;(c:case)
+OPTIONAL MATCH (f)--&gt;(parent)
+WITH f,a,ct,c,parent
+ WHERE f.file_format IN ['bai'] 
+ WITH
+    f, parent, c, a, ct,
+    ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+    toInteger(floor(log(f.file_size)/log(1024))) as i,
+    2 as precision
+WITH
+    f, parent, c, a, ct,
+    f.file_size /(1024^i) AS value,
+    10^precision AS factor,
+    units[i] as unit
+WITH
+    f, parent, c, a, ct, unit,
+    round(factor * value)/factor AS size
+RETURN DISTINCT
+    f.file_name AS `File Name`,
+    head(labels(parent)) as Association,
+    f.file_description AS Description,
+    f.file_format AS `File Format`,
+    CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+    ct.clinical_trial_designation AS `Trial Code`,
+    a.arm_id AS Arm,
+    c.case_id AS `Case ID`</t>
   </si>
 </sst>
 </file>
@@ -424,44 +483,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="75.81640625" customWidth="1"/>
-    <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
+    <row r="2" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>